<commit_message>
rework #23513, only use assimp for maths
</commit_message>
<xml_diff>
--- a/doc/S3D.xlsx
+++ b/doc/S3D.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n_seh\source\repos\Project4E53\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n_seh\source\repos\modelconvert\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D824BB62-BBDF-4E5D-8679-CD56264CC618}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B6D1CA-E09C-4F18-9419-6A82C967C587}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0A67637D-CBDB-4810-85E6-4DD9E363798E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>Data</t>
   </si>
@@ -156,13 +156,28 @@
     <t>Number of indices * uint (x * 4 byte)</t>
   </si>
   <si>
-    <t>Global armature inverse matrix</t>
-  </si>
-  <si>
     <t>Colors mark where</t>
   </si>
   <si>
     <t xml:space="preserve"> for loop is needed</t>
+  </si>
+  <si>
+    <t>char * root node string size</t>
+  </si>
+  <si>
+    <t>Node transform matrix</t>
+  </si>
+  <si>
+    <t>Num children</t>
+  </si>
+  <si>
+    <t>recursive</t>
+  </si>
+  <si>
+    <t>Node string size</t>
+  </si>
+  <si>
+    <t>Node string</t>
   </si>
 </sst>
 </file>
@@ -208,7 +223,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,6 +266,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -399,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -422,6 +443,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -736,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF7A8EB1-068F-4F5A-A84C-7C1C89E8289C}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,147 +801,145 @@
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D7" s="9"/>
       <c r="E7" s="5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>15</v>
-      </c>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" t="s">
         <v>42</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>43</v>
-      </c>
       <c r="D9" s="9"/>
       <c r="E9" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D10" s="9"/>
       <c r="E10" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D11" s="9"/>
+      <c r="D11" s="19"/>
       <c r="E11" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D12" s="21"/>
+      <c r="E12" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D13" s="21"/>
+      <c r="E13" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D14" s="21"/>
+      <c r="E14" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D12" s="19"/>
-      <c r="E12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="18"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="18"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="18"/>
-      <c r="E15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>25</v>
+      <c r="D15" s="21"/>
+      <c r="E15" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>4</v>
       </c>
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="18"/>
-      <c r="C16" s="17"/>
+      <c r="D16" s="13"/>
       <c r="E16" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="18"/>
-      <c r="C17" s="17"/>
+      <c r="D17" s="13"/>
       <c r="E17" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="18"/>
-      <c r="C18" s="17"/>
       <c r="E18" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G18" s="7"/>
     </row>
@@ -926,18 +947,20 @@
       <c r="B19" s="18"/>
       <c r="C19" s="17"/>
       <c r="E19" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="18"/>
       <c r="C20" s="17"/>
       <c r="E20" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>7</v>
@@ -947,50 +970,83 @@
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="18"/>
       <c r="C21" s="17"/>
-      <c r="D21" s="14"/>
       <c r="E21" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>38</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="G21" s="7"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="18"/>
       <c r="C22" s="17"/>
-      <c r="D22" s="14"/>
       <c r="E22" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="18"/>
+      <c r="C23" s="17"/>
+      <c r="E23" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="18"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="18"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F25" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G25" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D23" s="15"/>
-      <c r="E23" s="5" t="s">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D26" s="15"/>
+      <c r="E26" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F26" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G23" s="7"/>
-    </row>
-    <row r="24" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="15"/>
-      <c r="E24" s="10" t="s">
+      <c r="G26" s="7"/>
+    </row>
+    <row r="27" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="15"/>
+      <c r="E27" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F27" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="G24" s="12"/>
+      <c r="G27" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>